<commit_message>
add new experiments file
</commit_message>
<xml_diff>
--- a/Traceconstruction/benchmark/results-memory/experiments.xlsx
+++ b/Traceconstruction/benchmark/results-memory/experiments.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\araminit\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hojaji\Documents\GitHub\TraceCompaction\Traceconstruction\benchmark\results-memory\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="20490" windowHeight="6420" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Memory Results" sheetId="2" r:id="rId1"/>
@@ -327,7 +327,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.00000000000000%"/>
     <numFmt numFmtId="165" formatCode="#,##0.00&quot; &quot;[$€-40C];[Red]&quot;-&quot;#,##0.00&quot; &quot;[$€-40C]"/>
@@ -574,7 +574,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -726,7 +726,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-EB74-442D-B1A1-A510D67084EE}"/>
             </c:ext>
@@ -871,7 +871,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-EB74-442D-B1A1-A510D67084EE}"/>
             </c:ext>
@@ -887,11 +887,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="187608624"/>
-        <c:axId val="190724824"/>
+        <c:axId val="3896048"/>
+        <c:axId val="191421552"/>
       </c:barChart>
       <c:valAx>
-        <c:axId val="190724824"/>
+        <c:axId val="191421552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1004,12 +1004,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="187608624"/>
+        <c:crossAx val="3896048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="187608624"/>
+        <c:axId val="3896048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1098,7 +1098,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="190724824"/>
+        <c:crossAx val="191421552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1205,7 +1205,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1489,7 +1489,7 @@
             </c:numLit>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-FB38-43E0-BF04-265E4EE1DD4A}"/>
             </c:ext>
@@ -1503,8 +1503,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="188798600"/>
-        <c:axId val="189098920"/>
+        <c:axId val="186327536"/>
+        <c:axId val="156121352"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -1772,7 +1772,7 @@
             </c:numLit>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-FB38-43E0-BF04-265E4EE1DD4A}"/>
             </c:ext>
@@ -1786,11 +1786,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="191561784"/>
-        <c:axId val="192335216"/>
+        <c:axId val="192372192"/>
+        <c:axId val="66638192"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="189098920"/>
+        <c:axId val="156121352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1895,12 +1895,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="188798600"/>
+        <c:crossAx val="186327536"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="188798600"/>
+        <c:axId val="186327536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="180"/>
@@ -1998,12 +1998,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="189098920"/>
+        <c:crossAx val="156121352"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="192335216"/>
+        <c:axId val="66638192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2013,12 +2013,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="191561784"/>
+        <c:crossAx val="192372192"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="191561784"/>
+        <c:axId val="192372192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2028,7 +2028,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="192335216"/>
+        <c:crossAx val="66638192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2124,7 +2124,7 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2388,7 +2388,7 @@
             </c:numLit>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-0C0E-4D01-B877-DD89E5B2BEE6}"/>
             </c:ext>
@@ -2646,7 +2646,7 @@
             </c:numLit>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-0C0E-4D01-B877-DD89E5B2BEE6}"/>
             </c:ext>
@@ -2660,11 +2660,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="189531144"/>
-        <c:axId val="189530752"/>
+        <c:axId val="189015744"/>
+        <c:axId val="189015352"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="189530752"/>
+        <c:axId val="189015352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2777,12 +2777,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="189531144"/>
+        <c:crossAx val="189015744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="189531144"/>
+        <c:axId val="189015744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2872,7 +2872,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="189530752"/>
+        <c:crossAx val="189015352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2976,7 +2976,7 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3267,7 +3267,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-B3E7-4F10-872F-E6475FFC575D}"/>
             </c:ext>
@@ -3543,7 +3543,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-B3E7-4F10-872F-E6475FFC575D}"/>
             </c:ext>
@@ -3557,11 +3557,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="192811640"/>
-        <c:axId val="189531928"/>
+        <c:axId val="190978808"/>
+        <c:axId val="190978416"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="189531928"/>
+        <c:axId val="190978416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3617,12 +3617,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="192811640"/>
+        <c:crossAx val="190978808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="192811640"/>
+        <c:axId val="190978808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="200"/>
@@ -3679,7 +3679,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="189531928"/>
+        <c:crossAx val="190978416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3775,7 +3775,7 @@
 </file>
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3945,7 +3945,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-4AF1-4E6E-A227-4A9DA4FEAB6E}"/>
             </c:ext>
@@ -4105,7 +4105,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-4AF1-4E6E-A227-4A9DA4FEAB6E}"/>
             </c:ext>
@@ -4266,7 +4266,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-4AF1-4E6E-A227-4A9DA4FEAB6E}"/>
             </c:ext>
@@ -4282,11 +4282,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="192813600"/>
-        <c:axId val="192813208"/>
+        <c:axId val="190979984"/>
+        <c:axId val="190980376"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="192813600"/>
+        <c:axId val="190979984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4383,7 +4383,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="192813208"/>
+        <c:crossAx val="190980376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4391,7 +4391,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="192813208"/>
+        <c:axId val="190980376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4500,7 +4500,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="192813600"/>
+        <c:crossAx val="190979984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4591,7 +4591,7 @@
 </file>
 
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -4654,7 +4654,7 @@
                 <a:bevel/>
               </a:ln>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000000-D48A-42FB-9FDB-C8904AE81833}"/>
               </c:ext>
@@ -4684,7 +4684,7 @@
                 <a:miter/>
               </a:ln>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000001-D48A-42FB-9FDB-C8904AE81833}"/>
               </c:ext>
@@ -4714,7 +4714,7 @@
                 <a:miter/>
               </a:ln>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000002-D48A-42FB-9FDB-C8904AE81833}"/>
               </c:ext>
@@ -4743,7 +4743,7 @@
                 <a:miter/>
               </a:ln>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000003-D48A-42FB-9FDB-C8904AE81833}"/>
               </c:ext>
@@ -4796,16 +4796,16 @@
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
-              <c:extLst>
+              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-D48A-42FB-9FDB-C8904AE81833}"/>
+                </c:ext>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <a:prstGeom prst="rect">
                       <a:avLst/>
                     </a:prstGeom>
                   </c15:spPr>
-                </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000000-D48A-42FB-9FDB-C8904AE81833}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -4855,16 +4855,16 @@
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
-              <c:extLst>
+              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-D48A-42FB-9FDB-C8904AE81833}"/>
+                </c:ext>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <a:prstGeom prst="rect">
                       <a:avLst/>
                     </a:prstGeom>
                   </c15:spPr>
-                </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000001-D48A-42FB-9FDB-C8904AE81833}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -4914,16 +4914,16 @@
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
-              <c:extLst>
+              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-D48A-42FB-9FDB-C8904AE81833}"/>
+                </c:ext>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <a:prstGeom prst="rect">
                       <a:avLst/>
                     </a:prstGeom>
                   </c15:spPr>
-                </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000002-D48A-42FB-9FDB-C8904AE81833}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -4973,16 +4973,16 @@
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
-              <c:extLst>
+              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-D48A-42FB-9FDB-C8904AE81833}"/>
+                </c:ext>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <a:prstGeom prst="rect">
                       <a:avLst/>
                     </a:prstGeom>
                   </c15:spPr>
-                </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000003-D48A-42FB-9FDB-C8904AE81833}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -5025,7 +5025,7 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="1"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
           </c:dLbls>
@@ -5070,7 +5070,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000008-38F2-46BA-A6A8-5A2D5313C9BD}"/>
             </c:ext>
@@ -5178,7 +5178,7 @@
 </file>
 
 <file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -5243,7 +5243,7 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000000-B4D5-4834-BBFC-1C039A027D94}"/>
               </c:ext>
@@ -5267,7 +5267,7 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000001-B4D5-4834-BBFC-1C039A027D94}"/>
               </c:ext>
@@ -5291,7 +5291,7 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000002-B4D5-4834-BBFC-1C039A027D94}"/>
               </c:ext>
@@ -5315,7 +5315,7 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000003-B4D5-4834-BBFC-1C039A027D94}"/>
               </c:ext>
@@ -5371,7 +5371,7 @@
             <c:showBubbleSize val="0"/>
             <c:separator>, </c:separator>
             <c:showLeaderLines val="1"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <a:prstGeom prst="rect">
@@ -5422,7 +5422,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000008-FCF8-441D-B945-EFC3C39A1BFF}"/>
             </c:ext>
@@ -5534,7 +5534,7 @@
 </file>
 
 <file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -5630,7 +5630,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-D2E9-44B9-B8B9-4F8ED742114F}"/>
             </c:ext>
@@ -5702,7 +5702,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-D2E9-44B9-B8B9-4F8ED742114F}"/>
             </c:ext>
@@ -5774,7 +5774,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-D2E9-44B9-B8B9-4F8ED742114F}"/>
             </c:ext>
@@ -5846,7 +5846,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-D2E9-44B9-B8B9-4F8ED742114F}"/>
             </c:ext>
@@ -5918,7 +5918,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000004-D2E9-44B9-B8B9-4F8ED742114F}"/>
             </c:ext>
@@ -5935,11 +5935,11 @@
         </c:dLbls>
         <c:gapWidth val="79"/>
         <c:overlap val="100"/>
-        <c:axId val="192814776"/>
-        <c:axId val="192814384"/>
+        <c:axId val="190981552"/>
+        <c:axId val="190981160"/>
       </c:barChart>
       <c:valAx>
-        <c:axId val="192814384"/>
+        <c:axId val="190981160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6045,12 +6045,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="192814776"/>
+        <c:crossAx val="190981552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="192814776"/>
+        <c:axId val="190981552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6106,7 +6106,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="192814384"/>
+        <c:crossAx val="190981160"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13248,8 +13248,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="F13" workbookViewId="0">
+      <selection activeCell="M41" sqref="M41:M49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -15399,53 +15399,29 @@
       </c>
     </row>
     <row r="41" spans="1:15">
-      <c r="M41" s="36">
-        <f>1/(1-__Anonymous_Sheet_DB__04[[#This Row],[Column10]])</f>
-        <v>1</v>
-      </c>
+      <c r="M41" s="36"/>
     </row>
     <row r="42" spans="1:15">
-      <c r="M42" s="36">
-        <f>1/(1-__Anonymous_Sheet_DB__04[[#This Row],[Column10]])</f>
-        <v>1</v>
-      </c>
+      <c r="M42" s="36"/>
       <c r="O42" s="36"/>
     </row>
     <row r="43" spans="1:15">
-      <c r="M43" s="36">
-        <f>1/(1-__Anonymous_Sheet_DB__04[[#This Row],[Column10]])</f>
-        <v>1</v>
-      </c>
+      <c r="M43" s="36"/>
     </row>
     <row r="44" spans="1:15">
-      <c r="M44" s="36">
-        <f>1/(1-__Anonymous_Sheet_DB__04[[#This Row],[Column10]])</f>
-        <v>1</v>
-      </c>
+      <c r="M44" s="36"/>
     </row>
     <row r="45" spans="1:15">
-      <c r="M45" s="36">
-        <f>1/(1-__Anonymous_Sheet_DB__04[[#This Row],[Column10]])</f>
-        <v>1</v>
-      </c>
+      <c r="M45" s="36"/>
     </row>
     <row r="46" spans="1:15">
-      <c r="M46" s="36">
-        <f>1/(1-__Anonymous_Sheet_DB__04[[#This Row],[Column10]])</f>
-        <v>1</v>
-      </c>
+      <c r="M46" s="36"/>
     </row>
     <row r="47" spans="1:15">
-      <c r="M47" s="36">
-        <f>1/(1-__Anonymous_Sheet_DB__04[[#This Row],[Column10]])</f>
-        <v>1</v>
-      </c>
+      <c r="M47" s="36"/>
     </row>
     <row r="48" spans="1:15">
-      <c r="M48" s="36">
-        <f>1/(1-__Anonymous_Sheet_DB__04[[#This Row],[Column10]])</f>
-        <v>1</v>
-      </c>
+      <c r="M48" s="36"/>
     </row>
   </sheetData>
   <pageMargins left="0" right="0" top="0.39370078740157505" bottom="0.39370078740157505" header="0" footer="0"/>

</xml_diff>